<commit_message>
Added MPI Ethernet Graph
</commit_message>
<xml_diff>
--- a/times_and_speedups_excel_file.xlsx
+++ b/times_and_speedups_excel_file.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20" yWindow="860" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Before" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,15 @@
     <sheet name="MD_SEQ" sheetId="4" r:id="rId4"/>
     <sheet name="Ganhos vs SEQ" sheetId="5" r:id="rId5"/>
     <sheet name="Above 8" sheetId="6" r:id="rId6"/>
+    <sheet name="MPI_Ethernet" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
+    <definedName name="all_times_MPI" localSheetId="6">MPI_Ethernet!$A$1:$G$20</definedName>
     <definedName name="all_times_OMP" localSheetId="5">'Above 8'!$A$1:$E$15</definedName>
     <definedName name="all_times_OMP_1" localSheetId="1">After!$A$1:$E$10</definedName>
     <definedName name="all_times_SEQ" localSheetId="3">MD_SEQ!$A$1:$E$11</definedName>
   </definedNames>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -38,8 +40,21 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="all_times_OMP" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/Sergio/Desktop/Sergio/LEI/4Ano/CPD/2Semestre/AP/Trabalhos/TP3/AP_TP3_MD_Parallel/MD_OMP/results/time_results_OMP_after_auxs_var/all_times_OMP.csv" comma="1">
+  <connection id="1" name="all_times_MPI" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="/Users/Sergio/Desktop/Sergio/LEI/4Ano/CPD/2Semestre/AP/Trabalhos/TP3/AP_TP3_MD_Parallel/MD_MPI/time_results_MPI/results_4Nodes/all_times_MPI.csv" comma="1">
+      <textFields count="7">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" name="all_times_OMP" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/Sergio/Desktop/Sergio/LEI/4Ano/CPD/2Semestre/AP/Trabalhos/TP3/AP_TP3_MD_Parallel/MD_OMP/results/time_results_OMP_after_auxs_var/all_times_OMP.csv" comma="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -49,8 +64,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="all_times_OMP1" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/Sergio/Desktop/Sergio/LEI/4Ano/CPD/2Semestre/AP/Trabalhos/TP3/AP_TP3_MD_Parallel/MD_OMP/results/time_results_OMP_aux_var_above_8threads/all_times_OMP.csv" comma="1">
+  <connection id="3" name="all_times_OMP1" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/Sergio/Desktop/Sergio/LEI/4Ano/CPD/2Semestre/AP/Trabalhos/TP3/AP_TP3_MD_Parallel/MD_OMP/results/time_results_OMP_aux_var_above_8threads/all_times_OMP.csv" comma="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -60,8 +75,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="all_times_SEQ" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/Sergio/Desktop/Sergio/LEI/4Ano/CPD/2Semestre/AP/Trabalhos/TP3/AP_TP3_MD_Parallel/MD_SEQ/time_results_SEQ/all_times_SEQ.csv" comma="1">
+  <connection id="4" name="all_times_SEQ" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/Sergio/Desktop/Sergio/LEI/4Ano/CPD/2Semestre/AP/Trabalhos/TP3/AP_TP3_MD_Parallel/MD_SEQ/time_results_SEQ/all_times_SEQ.csv" comma="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -75,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="20">
   <si>
     <t>NODE</t>
   </si>
@@ -117,6 +132,24 @@
   </si>
   <si>
     <t>MD_SEQ</t>
+  </si>
+  <si>
+    <t>NNODES</t>
+  </si>
+  <si>
+    <t>MAPPED-BY</t>
+  </si>
+  <si>
+    <t>PPN</t>
+  </si>
+  <si>
+    <t>compute-641-3</t>
+  </si>
+  <si>
+    <t>MPI</t>
+  </si>
+  <si>
+    <t>core</t>
   </si>
 </sst>
 </file>
@@ -208,7 +241,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -292,9 +324,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -313,9 +343,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -334,9 +362,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -355,9 +381,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -376,9 +400,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -397,9 +419,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -418,9 +438,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -439,9 +457,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -460,9 +476,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -504,7 +518,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -598,7 +611,6 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -608,11 +620,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2115670224"/>
-        <c:axId val="2092647360"/>
+        <c:axId val="-2142782080"/>
+        <c:axId val="-2142779808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2115670224"/>
+        <c:axId val="-2142782080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -644,7 +656,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -710,7 +721,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2092647360"/>
+        <c:crossAx val="-2142779808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -718,7 +729,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2092647360"/>
+        <c:axId val="-2142779808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -741,7 +752,7 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -769,7 +780,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -779,7 +789,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
@@ -830,7 +840,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2115670224"/>
+        <c:crossAx val="-2142782080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1000.0"/>
@@ -845,7 +855,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -952,7 +961,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1036,9 +1044,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1057,9 +1063,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1078,9 +1082,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1099,9 +1101,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1120,9 +1120,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1141,9 +1139,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1162,9 +1158,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1183,9 +1177,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1204,9 +1196,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -1350,11 +1340,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2116370736"/>
-        <c:axId val="-2086901488"/>
+        <c:axId val="-2142674240"/>
+        <c:axId val="-2142668416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2116370736"/>
+        <c:axId val="-2142674240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1386,7 +1376,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1453,7 +1442,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2086901488"/>
+        <c:crossAx val="-2142668416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1461,7 +1450,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2086901488"/>
+        <c:axId val="-2142668416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1512,7 +1501,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1573,7 +1561,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2116370736"/>
+        <c:crossAx val="-2142674240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1000.0"/>
@@ -1588,7 +1576,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1700,7 +1687,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1783,9 +1769,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1803,9 +1787,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1823,9 +1805,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1843,9 +1823,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1863,9 +1841,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1883,9 +1859,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1903,9 +1877,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1923,9 +1895,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1943,9 +1913,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -1986,7 +1954,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2089,11 +2056,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2085935664"/>
-        <c:axId val="-2080695440"/>
+        <c:axId val="-2143735824"/>
+        <c:axId val="-2143730000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2085935664"/>
+        <c:axId val="-2143735824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2125,7 +2092,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2192,7 +2158,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2080695440"/>
+        <c:crossAx val="-2143730000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2200,7 +2166,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2080695440"/>
+        <c:axId val="-2143730000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5.0"/>
@@ -2248,7 +2214,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2309,7 +2274,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2085935664"/>
+        <c:crossAx val="-2143735824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.25"/>
@@ -2324,7 +2289,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2436,7 +2400,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2519,9 +2482,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -2539,9 +2500,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -2559,9 +2518,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -2579,9 +2536,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -2599,9 +2554,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -2619,9 +2572,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -2639,9 +2590,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -2659,9 +2608,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -2679,9 +2626,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -2824,11 +2769,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2088431856"/>
-        <c:axId val="-2082304096"/>
+        <c:axId val="-2143664224"/>
+        <c:axId val="-2143658400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2088431856"/>
+        <c:axId val="-2143664224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2860,7 +2805,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2927,7 +2871,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2082304096"/>
+        <c:crossAx val="-2143658400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2935,7 +2879,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2082304096"/>
+        <c:axId val="-2143658400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5.0"/>
@@ -2983,7 +2927,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3044,7 +2987,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2088431856"/>
+        <c:crossAx val="-2143664224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.25"/>
@@ -3059,7 +3002,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3557,7 +3499,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3704,11 +3645,11 @@
         </c:dropLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2086443248"/>
-        <c:axId val="-2080913376"/>
+        <c:axId val="-2143585440"/>
+        <c:axId val="-2143579712"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2086443248"/>
+        <c:axId val="-2143585440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3807,7 +3748,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2080913376"/>
+        <c:crossAx val="-2143579712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3815,7 +3756,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2080913376"/>
+        <c:axId val="-2143579712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3927,10 +3868,1016 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2086443248"/>
+        <c:crossAx val="-2143585440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1000.0"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Times</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> for MD_MPI Kernel with Ethernet</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>MD_MPI_Ethernet</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0271317829457364"/>
+                  <c:y val="-0.0253807106598986"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0245478036175711"/>
+                  <c:y val="-0.0219966159052453"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0245478036175711"/>
+                  <c:y val="-0.0236886632825719"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0271317829457365"/>
+                  <c:y val="-0.0253807106598985"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0322997416020672"/>
+                  <c:y val="-0.0219966159052455"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0348837209302326"/>
+                  <c:y val="-0.0219966159052453"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0322997416020672"/>
+                  <c:y val="-0.0219966159052453"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0348837209302325"/>
+                  <c:y val="-0.0253807106598986"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0400516795865633"/>
+                  <c:y val="-0.0253807106598986"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0348837209302326"/>
+                  <c:y val="-0.0270727580372252"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0387596899224807"/>
+                  <c:y val="-0.027072758037225"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="11"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0490956072351421"/>
+                  <c:y val="-0.0236886632825719"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="12"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0465116279069768"/>
+                  <c:y val="-0.011844331641286"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="13"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0503875968992249"/>
+                  <c:y val="-0.027072758037225"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="14"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0322997416020672"/>
+                  <c:y val="-0.023688663282572"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="15"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0232558139534884"/>
+                  <c:y val="0.0219966159052453"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="16"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.00516795865633084"/>
+                  <c:y val="0.00507614213197963"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="17"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.00516795865633075"/>
+                  <c:y val="0.00676818950930623"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="18"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.00775193798449612"/>
+                  <c:y val="0.00507614213197969"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>MPI_Ethernet!$F$2:$F$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>34.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>128.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>MPI_Ethernet!$G$2:$G$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1465.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1503.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1565.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1662.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1691.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1707.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1758.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1767.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2457.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2613.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2555.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2716.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7032.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11201.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>12057.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10046.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10711.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>14459.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18185.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:dropLines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="35000"/>
+                  <a:lumOff val="65000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:dropLines>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2100765808"/>
+        <c:axId val="-2102616944"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2100765808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Nº Processes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2102616944"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2102616944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="19000.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2100765808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="500.0"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -4209,6 +5156,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -6222,6 +7209,509 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6907,16 +8397,55 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="all_times_OMP_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="all_times_OMP_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="all_times_SEQ" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="all_times_SEQ" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="all_times_OMP" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="all_times_OMP" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="all_times_MPI" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8106,7 +9635,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
@@ -8382,4 +9911,492 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="F12" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1465</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>1503</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>1565</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>8</v>
+      </c>
+      <c r="G5">
+        <v>1662</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <v>1691</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>12</v>
+      </c>
+      <c r="G7">
+        <v>1707</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>14</v>
+      </c>
+      <c r="G8">
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>16</v>
+      </c>
+      <c r="G9">
+        <v>1767</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>22</v>
+      </c>
+      <c r="G10">
+        <v>2457</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>24</v>
+      </c>
+      <c r="G11">
+        <v>2613</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>26</v>
+      </c>
+      <c r="G12">
+        <v>2555</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>28</v>
+      </c>
+      <c r="G13">
+        <v>2716</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>30</v>
+      </c>
+      <c r="G14">
+        <v>7032</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>32</v>
+      </c>
+      <c r="G15">
+        <v>11201</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>34</v>
+      </c>
+      <c r="G16">
+        <v>12057</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>36</v>
+      </c>
+      <c r="G17">
+        <v>10046</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>38</v>
+      </c>
+      <c r="G18">
+        <v>10711</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>64</v>
+      </c>
+      <c r="G19">
+        <v>14459</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>128</v>
+      </c>
+      <c r="G20">
+        <v>18185</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="F2:G96">
+    <sortCondition ref="F2:F96"/>
+    <sortCondition ref="G2:G96"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>